<commit_message>
Added icons for construction, transport, accomodation and communication
</commit_message>
<xml_diff>
--- a/NaceCodes.xlsx
+++ b/NaceCodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9645"/>
   </bookViews>
   <sheets>
     <sheet name="NACE_REV2_20170420_094836" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NACE_REV2_20170420_094836!$A$1:$J$997</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -15308,8 +15308,8 @@
   <dimension ref="A1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A458" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E489" sqref="E489"/>
+      <pane ySplit="1" topLeftCell="A674" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E685" sqref="E685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15768,7 +15768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>398498</v>
       </c>
@@ -17670,7 +17670,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>398573</v>
       </c>
@@ -18258,7 +18258,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>398596</v>
       </c>
@@ -18691,7 +18691,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>398612</v>
       </c>
@@ -19905,7 +19905,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>398661</v>
       </c>
@@ -21297,7 +21297,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>398716</v>
       </c>
@@ -28024,7 +28024,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A506">
         <v>398985</v>
       </c>
@@ -28050,7 +28050,7 @@
         <v>1711</v>
       </c>
     </row>
-    <row r="507" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A507">
         <v>398986</v>
       </c>
@@ -28070,7 +28070,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="508" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>398987</v>
       </c>
@@ -28099,7 +28099,7 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="509" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A509">
         <v>398988</v>
       </c>
@@ -28119,7 +28119,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A510">
         <v>398989</v>
       </c>
@@ -28148,7 +28148,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="511" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>398990</v>
       </c>
@@ -28177,7 +28177,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="512" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A512">
         <v>398991</v>
       </c>
@@ -28197,7 +28197,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A513">
         <v>398992</v>
       </c>
@@ -28228,7 +28228,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="514" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A514">
         <v>398993</v>
       </c>
@@ -28251,7 +28251,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="515" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A515">
         <v>398994</v>
       </c>
@@ -28271,7 +28271,7 @@
         <v>4530</v>
       </c>
     </row>
-    <row r="516" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A516">
         <v>398995</v>
       </c>
@@ -28294,7 +28294,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A517">
         <v>398996</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="518" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A518">
         <v>398997</v>
       </c>
@@ -28340,7 +28340,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="519" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A519">
         <v>398998</v>
       </c>
@@ -28366,7 +28366,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="520" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A520">
         <v>398999</v>
       </c>
@@ -28392,7 +28392,7 @@
         <v>1758</v>
       </c>
     </row>
-    <row r="521" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A521">
         <v>399000</v>
       </c>
@@ -28415,7 +28415,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="522" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A522">
         <v>399001</v>
       </c>
@@ -28441,7 +28441,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="523" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A523">
         <v>399002</v>
       </c>
@@ -28464,7 +28464,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="524" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A524">
         <v>399003</v>
       </c>
@@ -28490,7 +28490,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="525" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A525">
         <v>399004</v>
       </c>
@@ -28513,7 +28513,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="526" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A526">
         <v>399005</v>
       </c>
@@ -28536,7 +28536,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="527" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A527">
         <v>399006</v>
       </c>
@@ -28559,7 +28559,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="528" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A528">
         <v>399007</v>
       </c>
@@ -28582,7 +28582,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="529" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A529">
         <v>399008</v>
       </c>
@@ -28605,7 +28605,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="530" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A530">
         <v>399009</v>
       </c>
@@ -28625,7 +28625,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="531" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A531">
         <v>399010</v>
       </c>
@@ -28651,7 +28651,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="532" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A532">
         <v>399011</v>
       </c>
@@ -28674,7 +28674,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="533" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A533">
         <v>399012</v>
       </c>
@@ -28694,7 +28694,7 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="534" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A534">
         <v>399013</v>
       </c>
@@ -28714,7 +28714,7 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="535" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A535">
         <v>399014</v>
       </c>
@@ -28734,7 +28734,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="536" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A536">
         <v>399015</v>
       </c>
@@ -28757,7 +28757,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="537" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A537">
         <v>399016</v>
       </c>
@@ -28777,7 +28777,7 @@
         <v>4630</v>
       </c>
     </row>
-    <row r="538" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A538">
         <v>399017</v>
       </c>
@@ -28800,7 +28800,7 @@
         <v>1804</v>
       </c>
     </row>
-    <row r="539" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A539">
         <v>399018</v>
       </c>
@@ -28829,7 +28829,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="540" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A540">
         <v>399019</v>
       </c>
@@ -28849,7 +28849,7 @@
         <v>4630</v>
       </c>
     </row>
-    <row r="541" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A541">
         <v>399020</v>
       </c>
@@ -28876,7 +28876,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="542" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A542">
         <v>399021</v>
       </c>
@@ -28896,7 +28896,7 @@
         <v>4630</v>
       </c>
     </row>
-    <row r="543" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A543">
         <v>399022</v>
       </c>
@@ -28919,7 +28919,7 @@
         <v>1819</v>
       </c>
     </row>
-    <row r="544" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A544">
         <v>399023</v>
       </c>
@@ -28939,7 +28939,7 @@
         <v>4630</v>
       </c>
     </row>
-    <row r="545" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A545">
         <v>399024</v>
       </c>
@@ -28962,7 +28962,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="546" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A546">
         <v>399025</v>
       </c>
@@ -28988,7 +28988,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="547" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A547">
         <v>399026</v>
       </c>
@@ -29014,7 +29014,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="548" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A548">
         <v>399027</v>
       </c>
@@ -29040,7 +29040,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="549" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A549">
         <v>399028</v>
       </c>
@@ -29063,7 +29063,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="550" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A550">
         <v>399029</v>
       </c>
@@ -29086,7 +29086,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="551" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A551">
         <v>399030</v>
       </c>
@@ -29109,7 +29109,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="552" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A552">
         <v>399031</v>
       </c>
@@ -29135,7 +29135,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="553" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553">
         <v>399032</v>
       </c>
@@ -29155,7 +29155,7 @@
         <v>4649</v>
       </c>
     </row>
-    <row r="554" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A554">
         <v>399033</v>
       </c>
@@ -29182,7 +29182,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="555" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555">
         <v>399034</v>
       </c>
@@ -29205,7 +29205,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="556" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A556">
         <v>399035</v>
       </c>
@@ -29235,7 +29235,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="557" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A557">
         <v>399036</v>
       </c>
@@ -29261,7 +29261,7 @@
         <v>1864</v>
       </c>
     </row>
-    <row r="558" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A558">
         <v>399037</v>
       </c>
@@ -29284,7 +29284,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="559" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A559">
         <v>399038</v>
       </c>
@@ -29310,7 +29310,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="560" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A560">
         <v>399039</v>
       </c>
@@ -29336,7 +29336,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="561" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A561">
         <v>399040</v>
       </c>
@@ -29356,7 +29356,7 @@
         <v>4659</v>
       </c>
     </row>
-    <row r="562" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A562">
         <v>399041</v>
       </c>
@@ -29379,7 +29379,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="563" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A563">
         <v>399042</v>
       </c>
@@ -29402,7 +29402,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="564" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A564">
         <v>399043</v>
       </c>
@@ -29428,7 +29428,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="565" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A565">
         <v>399044</v>
       </c>
@@ -29461,7 +29461,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="566" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A566">
         <v>399045</v>
       </c>
@@ -29484,7 +29484,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="567" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A567">
         <v>399046</v>
       </c>
@@ -29507,7 +29507,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="568" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A568">
         <v>399047</v>
       </c>
@@ -29536,7 +29536,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="569" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A569">
         <v>399048</v>
       </c>
@@ -29559,7 +29559,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="570" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A570">
         <v>399049</v>
       </c>
@@ -29582,7 +29582,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="571" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A571">
         <v>399050</v>
       </c>
@@ -29605,7 +29605,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="572" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A572">
         <v>399051</v>
       </c>
@@ -29628,7 +29628,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="573" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A573">
         <v>399052</v>
       </c>
@@ -29657,7 +29657,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="574" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A574">
         <v>399053</v>
       </c>
@@ -29677,7 +29677,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="575" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A575">
         <v>399054</v>
       </c>
@@ -29700,7 +29700,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="576" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A576">
         <v>399055</v>
       </c>
@@ -29729,7 +29729,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="577" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A577">
         <v>399056</v>
       </c>
@@ -29752,7 +29752,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="578" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A578">
         <v>399057</v>
       </c>
@@ -29775,7 +29775,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="579" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A579">
         <v>399058</v>
       </c>
@@ -29798,7 +29798,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="580" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A580">
         <v>399059</v>
       </c>
@@ -29818,7 +29818,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="581" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A581">
         <v>399060</v>
       </c>
@@ -29841,7 +29841,7 @@
         <v>1942</v>
       </c>
     </row>
-    <row r="582" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A582">
         <v>399061</v>
       </c>
@@ -29864,7 +29864,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="583" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A583">
         <v>399062</v>
       </c>
@@ -29887,7 +29887,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="584" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A584">
         <v>399063</v>
       </c>
@@ -29911,7 +29911,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="585" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A585">
         <v>399064</v>
       </c>
@@ -29934,7 +29934,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="586" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A586">
         <v>399065</v>
       </c>
@@ -29957,7 +29957,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="587" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A587">
         <v>399066</v>
       </c>
@@ -29980,7 +29980,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="588" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A588">
         <v>399067</v>
       </c>
@@ -30000,7 +30000,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="589" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A589">
         <v>399068</v>
       </c>
@@ -30029,7 +30029,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="590" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A590">
         <v>399069</v>
       </c>
@@ -30052,7 +30052,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="591" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A591">
         <v>399070</v>
       </c>
@@ -30078,7 +30078,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="592" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A592">
         <v>399071</v>
       </c>
@@ -30098,7 +30098,7 @@
         <v>4741</v>
       </c>
     </row>
-    <row r="593" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A593">
         <v>399072</v>
       </c>
@@ -30121,7 +30121,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="594" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A594">
         <v>399073</v>
       </c>
@@ -30144,7 +30144,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="595" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A595">
         <v>399074</v>
       </c>
@@ -30170,7 +30170,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="596" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A596">
         <v>399075</v>
       </c>
@@ -30200,7 +30200,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="597" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A597">
         <v>399076</v>
       </c>
@@ -30226,7 +30226,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="598" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A598">
         <v>399077</v>
       </c>
@@ -30249,7 +30249,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="599" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A599">
         <v>399078</v>
       </c>
@@ -30275,7 +30275,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="600" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A600">
         <v>399079</v>
       </c>
@@ -30298,7 +30298,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="601" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A601">
         <v>399080</v>
       </c>
@@ -30324,7 +30324,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="602" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A602">
         <v>399081</v>
       </c>
@@ -30347,7 +30347,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="603" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A603">
         <v>399082</v>
       </c>
@@ -30373,7 +30373,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="604" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A604">
         <v>399083</v>
       </c>
@@ -30396,7 +30396,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="605" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A605">
         <v>399084</v>
       </c>
@@ -30422,7 +30422,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="606" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A606">
         <v>399085</v>
       </c>
@@ -30448,7 +30448,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="607" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A607">
         <v>399086</v>
       </c>
@@ -30474,7 +30474,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="608" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A608">
         <v>399087</v>
       </c>
@@ -30500,7 +30500,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="609" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A609">
         <v>399088</v>
       </c>
@@ -30523,7 +30523,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="610" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A610">
         <v>399089</v>
       </c>
@@ -30543,7 +30543,7 @@
         <v>4772</v>
       </c>
     </row>
-    <row r="611" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A611">
         <v>399090</v>
       </c>
@@ -30566,7 +30566,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="612" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A612">
         <v>399091</v>
       </c>
@@ -30586,7 +30586,7 @@
         <v>4773</v>
       </c>
     </row>
-    <row r="613" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A613">
         <v>399092</v>
       </c>
@@ -30606,7 +30606,7 @@
         <v>4773</v>
       </c>
     </row>
-    <row r="614" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A614">
         <v>399093</v>
       </c>
@@ -30629,7 +30629,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="615" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A615">
         <v>399094</v>
       </c>
@@ -30655,7 +30655,7 @@
         <v>2051</v>
       </c>
     </row>
-    <row r="616" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A616">
         <v>399095</v>
       </c>
@@ -30678,7 +30678,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="617" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A617">
         <v>399096</v>
       </c>
@@ -30701,7 +30701,7 @@
         <v>2057</v>
       </c>
     </row>
-    <row r="618" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A618">
         <v>399097</v>
       </c>
@@ -30721,7 +30721,7 @@
         <v>4782</v>
       </c>
     </row>
-    <row r="619" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A619">
         <v>399098</v>
       </c>
@@ -30744,7 +30744,7 @@
         <v>2062</v>
       </c>
     </row>
-    <row r="620" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A620">
         <v>399099</v>
       </c>
@@ -30767,7 +30767,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="621" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A621">
         <v>399100</v>
       </c>
@@ -30799,7 +30799,7 @@
         <v>2071</v>
       </c>
     </row>
-    <row r="622" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A622">
         <v>399101</v>
       </c>
@@ -30826,7 +30826,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="623" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A623">
         <v>399102</v>
       </c>
@@ -30849,7 +30849,7 @@
         <v>2078</v>
       </c>
     </row>
-    <row r="624" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A624">
         <v>399103</v>
       </c>
@@ -30872,7 +30872,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="625" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A625">
         <v>399104</v>
       </c>
@@ -30892,7 +30892,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="626" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A626">
         <v>399105</v>
       </c>
@@ -30918,7 +30918,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="627" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A627">
         <v>399106</v>
       </c>
@@ -30938,7 +30938,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="628" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A628">
         <v>399107</v>
       </c>
@@ -30964,7 +30964,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="629" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A629">
         <v>399108</v>
       </c>
@@ -30987,7 +30987,7 @@
         <v>2093</v>
       </c>
     </row>
-    <row r="630" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A630">
         <v>399109</v>
       </c>
@@ -31016,7 +31016,7 @@
         <v>2098</v>
       </c>
     </row>
-    <row r="631" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="631" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A631">
         <v>399110</v>
       </c>
@@ -31044,7 +31044,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="632" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="632" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A632">
         <v>399111</v>
       </c>
@@ -31077,7 +31077,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="633" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="633" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A633">
         <v>399112</v>
       </c>
@@ -31100,7 +31100,7 @@
         <v>2109</v>
       </c>
     </row>
-    <row r="634" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A634">
         <v>399113</v>
       </c>
@@ -31132,7 +31132,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="635" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A635">
         <v>399114</v>
       </c>
@@ -31155,7 +31155,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="636" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A636">
         <v>399115</v>
       </c>
@@ -31175,7 +31175,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="637" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A637">
         <v>399116</v>
       </c>
@@ -31204,7 +31204,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="638" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="638" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A638">
         <v>399117</v>
       </c>
@@ -31230,7 +31230,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="639" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A639">
         <v>399118</v>
       </c>
@@ -31256,7 +31256,7 @@
         <v>2131</v>
       </c>
     </row>
-    <row r="640" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="640" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A640">
         <v>399119</v>
       </c>
@@ -31289,7 +31289,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="641" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A641">
         <v>399120</v>
       </c>
@@ -31315,7 +31315,7 @@
         <v>2139</v>
       </c>
     </row>
-    <row r="642" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A642">
         <v>399121</v>
       </c>
@@ -31348,7 +31348,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="643" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A643">
         <v>399122</v>
       </c>
@@ -31371,7 +31371,7 @@
         <v>2146</v>
       </c>
     </row>
-    <row r="644" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A644">
         <v>399123</v>
       </c>
@@ -31400,7 +31400,7 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="645" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A645">
         <v>399124</v>
       </c>
@@ -31423,7 +31423,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="646" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A646">
         <v>399125</v>
       </c>
@@ -31452,7 +31452,7 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="647" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A647">
         <v>399126</v>
       </c>
@@ -31478,7 +31478,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="648" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A648">
         <v>399127</v>
       </c>
@@ -31498,7 +31498,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="649" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A649">
         <v>399128</v>
       </c>
@@ -31527,7 +31527,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="650" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A650">
         <v>399129</v>
       </c>
@@ -31547,7 +31547,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="651" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A651">
         <v>399130</v>
       </c>
@@ -31573,7 +31573,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="652" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A652">
         <v>399131</v>
       </c>
@@ -31596,7 +31596,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="653" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A653">
         <v>399132</v>
       </c>
@@ -31619,7 +31619,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="654" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A654">
         <v>399133</v>
       </c>
@@ -31639,7 +31639,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="655" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A655">
         <v>399134</v>
       </c>
@@ -31672,7 +31672,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="656" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A656">
         <v>399135</v>
       </c>
@@ -31695,7 +31695,7 @@
         <v>2186</v>
       </c>
     </row>
-    <row r="657" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A657">
         <v>399136</v>
       </c>
@@ -31731,7 +31731,7 @@
         <v>2191</v>
       </c>
     </row>
-    <row r="658" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A658">
         <v>399137</v>
       </c>
@@ -31761,7 +31761,7 @@
         <v>2195</v>
       </c>
     </row>
-    <row r="659" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A659">
         <v>399138</v>
       </c>
@@ -31793,7 +31793,7 @@
         <v>2201</v>
       </c>
     </row>
-    <row r="660" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A660">
         <v>399139</v>
       </c>
@@ -31822,7 +31822,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="661" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A661">
         <v>399140</v>
       </c>
@@ -31848,7 +31848,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="662" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A662">
         <v>399141</v>
       </c>
@@ -31874,7 +31874,7 @@
         <v>2213</v>
       </c>
     </row>
-    <row r="663" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A663">
         <v>399142</v>
       </c>
@@ -31894,7 +31894,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="664" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A664">
         <v>399143</v>
       </c>
@@ -31920,7 +31920,7 @@
         <v>2218</v>
       </c>
     </row>
-    <row r="665" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A665">
         <v>399144</v>
       </c>
@@ -31940,7 +31940,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="666" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A666">
         <v>399145</v>
       </c>
@@ -31969,7 +31969,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="667" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A667">
         <v>399146</v>
       </c>
@@ -31992,7 +31992,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="668" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>399147</v>
       </c>
@@ -32021,7 +32021,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="669" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A669">
         <v>399148</v>
       </c>
@@ -32041,7 +32041,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="670" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A670">
         <v>399149</v>
       </c>
@@ -32070,7 +32070,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="671" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A671">
         <v>399150</v>
       </c>
@@ -32090,7 +32090,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="672" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A672">
         <v>399151</v>
       </c>
@@ -32119,7 +32119,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="673" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A673">
         <v>399152</v>
       </c>
@@ -32139,7 +32139,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="674" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A674">
         <v>399153</v>
       </c>
@@ -32168,7 +32168,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="675" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>399154</v>
       </c>
@@ -32188,7 +32188,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="676" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A676">
         <v>399155</v>
       </c>
@@ -32211,7 +32211,7 @@
         <v>2254</v>
       </c>
     </row>
-    <row r="677" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A677">
         <v>399156</v>
       </c>
@@ -32237,7 +32237,7 @@
         <v>2257</v>
       </c>
     </row>
-    <row r="678" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A678">
         <v>399157</v>
       </c>
@@ -32257,7 +32257,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="679" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A679">
         <v>399158</v>
       </c>
@@ -32289,7 +32289,7 @@
         <v>2264</v>
       </c>
     </row>
-    <row r="680" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A680">
         <v>399159</v>
       </c>
@@ -32312,7 +32312,7 @@
         <v>2267</v>
       </c>
     </row>
-    <row r="681" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A681">
         <v>399160</v>
       </c>
@@ -32338,7 +32338,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="682" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A682">
         <v>399161</v>
       </c>
@@ -32364,7 +32364,7 @@
         <v>2271</v>
       </c>
     </row>
-    <row r="683" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A683">
         <v>399162</v>
       </c>
@@ -32384,7 +32384,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="684" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A684">
         <v>399163</v>
       </c>
@@ -32410,7 +32410,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="685" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A685">
         <v>399164</v>
       </c>
@@ -32430,7 +32430,7 @@
         <v>2282</v>
       </c>
     </row>
-    <row r="686" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A686">
         <v>399165</v>
       </c>
@@ -32456,7 +32456,7 @@
         <v>2285</v>
       </c>
     </row>
-    <row r="687" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A687">
         <v>399166</v>
       </c>
@@ -32479,7 +32479,7 @@
         <v>2288</v>
       </c>
     </row>
-    <row r="688" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A688">
         <v>399167</v>
       </c>
@@ -32505,7 +32505,7 @@
         <v>2292</v>
       </c>
     </row>
-    <row r="689" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A689">
         <v>399168</v>
       </c>
@@ -32528,7 +32528,7 @@
         <v>2295</v>
       </c>
     </row>
-    <row r="690" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A690">
         <v>399169</v>
       </c>
@@ -32554,7 +32554,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="691" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A691">
         <v>399170</v>
       </c>
@@ -32577,7 +32577,7 @@
         <v>2302</v>
       </c>
     </row>
-    <row r="692" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A692">
         <v>399171</v>
       </c>
@@ -32607,7 +32607,7 @@
         <v>2306</v>
       </c>
     </row>
-    <row r="693" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A693">
         <v>399172</v>
       </c>
@@ -32627,7 +32627,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="694" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A694">
         <v>399173</v>
       </c>
@@ -32654,7 +32654,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="695" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A695">
         <v>399174</v>
       </c>
@@ -32684,7 +32684,7 @@
         <v>2315</v>
       </c>
     </row>
-    <row r="696" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A696">
         <v>399175</v>
       </c>
@@ -32710,7 +32710,7 @@
         <v>2318</v>
       </c>
     </row>
-    <row r="697" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A697">
         <v>399176</v>
       </c>
@@ -32736,7 +32736,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="698" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A698">
         <v>399177</v>
       </c>
@@ -32762,7 +32762,7 @@
         <v>2326</v>
       </c>
     </row>
-    <row r="699" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A699">
         <v>399178</v>
       </c>
@@ -32791,7 +32791,7 @@
         <v>2331</v>
       </c>
     </row>
-    <row r="700" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A700">
         <v>399179</v>
       </c>
@@ -32820,7 +32820,7 @@
         <v>2336</v>
       </c>
     </row>
-    <row r="701" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A701">
         <v>399180</v>
       </c>
@@ -32843,7 +32843,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="702" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A702">
         <v>399181</v>
       </c>
@@ -32863,7 +32863,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="703" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A703">
         <v>399182</v>
       </c>
@@ -32889,7 +32889,7 @@
         <v>2344</v>
       </c>
     </row>
-    <row r="704" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A704">
         <v>399183</v>
       </c>
@@ -32918,7 +32918,7 @@
         <v>2348</v>
       </c>
     </row>
-    <row r="705" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A705">
         <v>399184</v>
       </c>
@@ -32938,7 +32938,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="706" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A706">
         <v>399185</v>
       </c>
@@ -32967,7 +32967,7 @@
         <v>2354</v>
       </c>
     </row>
-    <row r="707" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A707">
         <v>399186</v>
       </c>
@@ -32987,7 +32987,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="708" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A708">
         <v>399187</v>
       </c>
@@ -33020,7 +33020,7 @@
         <v>2360</v>
       </c>
     </row>
-    <row r="709" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A709">
         <v>399188</v>
       </c>
@@ -33043,7 +33043,7 @@
         <v>2362</v>
       </c>
     </row>
-    <row r="710" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A710">
         <v>399189</v>
       </c>
@@ -33063,7 +33063,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="711" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A711">
         <v>399190</v>
       </c>
@@ -33092,7 +33092,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="712" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A712">
         <v>399191</v>
       </c>
@@ -33112,7 +33112,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="713" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A713">
         <v>399192</v>
       </c>
@@ -33141,7 +33141,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="714" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A714">
         <v>399193</v>
       </c>
@@ -33161,7 +33161,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="715" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A715">
         <v>399194</v>
       </c>
@@ -33190,7 +33190,7 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="716" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="716" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A716">
         <v>399195</v>
       </c>
@@ -33210,7 +33210,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="717" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="717" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A717">
         <v>399196</v>
       </c>
@@ -33243,7 +33243,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="718" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A718">
         <v>399197</v>
       </c>
@@ -33266,7 +33266,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="719" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A719">
         <v>399198</v>
       </c>
@@ -33286,7 +33286,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="720" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A720">
         <v>399199</v>
       </c>
@@ -33312,7 +33312,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="721" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A721">
         <v>399200</v>
       </c>
@@ -33338,7 +33338,7 @@
         <v>2394</v>
       </c>
     </row>
-    <row r="722" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="722" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A722">
         <v>399201</v>
       </c>
@@ -33361,7 +33361,7 @@
         <v>2397</v>
       </c>
     </row>
-    <row r="723" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A723">
         <v>399202</v>
       </c>
@@ -33387,7 +33387,7 @@
         <v>2401</v>
       </c>
     </row>
-    <row r="724" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A724">
         <v>399203</v>
       </c>
@@ -33410,7 +33410,7 @@
         <v>2403</v>
       </c>
     </row>
-    <row r="725" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A725">
         <v>399204</v>
       </c>
@@ -33433,7 +33433,7 @@
         <v>2406</v>
       </c>
     </row>
-    <row r="726" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A726">
         <v>399205</v>
       </c>
@@ -33459,7 +33459,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="727" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A727">
         <v>399206</v>
       </c>
@@ -33485,7 +33485,7 @@
         <v>2414</v>
       </c>
     </row>
-    <row r="728" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A728">
         <v>399207</v>
       </c>
@@ -33511,7 +33511,7 @@
         <v>2418</v>
       </c>
     </row>
-    <row r="729" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A729">
         <v>399208</v>
       </c>
@@ -33537,7 +33537,7 @@
         <v>2422</v>
       </c>
     </row>
-    <row r="730" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A730">
         <v>399209</v>
       </c>
@@ -33567,7 +33567,7 @@
         <v>2426</v>
       </c>
     </row>
-    <row r="731" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A731">
         <v>399210</v>
       </c>
@@ -33590,7 +33590,7 @@
         <v>2430</v>
       </c>
     </row>
-    <row r="732" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="732" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A732">
         <v>399211</v>
       </c>
@@ -33613,7 +33613,7 @@
         <v>2432</v>
       </c>
     </row>
-    <row r="733" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A733">
         <v>399212</v>
       </c>
@@ -33636,7 +33636,7 @@
         <v>2435</v>
       </c>
     </row>
-    <row r="734" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A734">
         <v>399213</v>
       </c>
@@ -33659,7 +33659,7 @@
         <v>2438</v>
       </c>
     </row>
-    <row r="735" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A735">
         <v>399214</v>
       </c>
@@ -33692,7 +33692,7 @@
         <v>2443</v>
       </c>
     </row>
-    <row r="736" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A736">
         <v>399215</v>
       </c>
@@ -33712,7 +33712,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="737" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="737" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A737">
         <v>399216</v>
       </c>
@@ -33738,7 +33738,7 @@
         <v>2448</v>
       </c>
     </row>
-    <row r="738" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A738">
         <v>399217</v>
       </c>
@@ -33758,7 +33758,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="739" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A739">
         <v>399218</v>
       </c>
@@ -33784,7 +33784,7 @@
         <v>2453</v>
       </c>
     </row>
-    <row r="740" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A740">
         <v>399219</v>
       </c>
@@ -33810,7 +33810,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="741" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="741" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A741">
         <v>399220</v>
       </c>
@@ -33836,7 +33836,7 @@
         <v>2461</v>
       </c>
     </row>
-    <row r="742" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A742">
         <v>399221</v>
       </c>
@@ -33862,7 +33862,7 @@
         <v>2465</v>
       </c>
     </row>
-    <row r="743" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="743" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A743">
         <v>399222</v>
       </c>
@@ -33891,7 +33891,7 @@
         <v>2470</v>
       </c>
     </row>
-    <row r="744" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A744">
         <v>399223</v>
       </c>
@@ -33914,7 +33914,7 @@
         <v>2472</v>
       </c>
     </row>
-    <row r="745" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="745" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A745">
         <v>399224</v>
       </c>
@@ -33937,7 +33937,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="746" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A746">
         <v>399225</v>
       </c>
@@ -33964,7 +33964,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="747" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="747" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A747">
         <v>399226</v>
       </c>
@@ -33992,7 +33992,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="748" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A748">
         <v>399227</v>
       </c>
@@ -34012,7 +34012,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="749" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="749" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A749">
         <v>399228</v>
       </c>
@@ -34035,7 +34035,7 @@
         <v>2485</v>
       </c>
     </row>
-    <row r="750" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A750">
         <v>399229</v>
       </c>
@@ -34055,7 +34055,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="751" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="751" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A751">
         <v>399230</v>
       </c>
@@ -34085,7 +34085,7 @@
         <v>2490</v>
       </c>
     </row>
-    <row r="752" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="752" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A752">
         <v>399231</v>
       </c>
@@ -34108,7 +34108,7 @@
         <v>2492</v>
       </c>
     </row>
-    <row r="753" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="753" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A753">
         <v>399232</v>
       </c>
@@ -34131,7 +34131,7 @@
         <v>2495</v>
       </c>
     </row>
-    <row r="754" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A754">
         <v>399233</v>
       </c>
@@ -34154,7 +34154,7 @@
         <v>2498</v>
       </c>
     </row>
-    <row r="755" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="755" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A755">
         <v>399234</v>
       </c>
@@ -34185,7 +34185,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="756" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="756" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A756">
         <v>399235</v>
       </c>
@@ -34220,7 +34220,7 @@
         <v>2507</v>
       </c>
     </row>
-    <row r="757" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="757" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A757">
         <v>399236</v>
       </c>
@@ -34243,7 +34243,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="758" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="758" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A758">
         <v>399237</v>
       </c>
@@ -34273,7 +34273,7 @@
         <v>2514</v>
       </c>
     </row>
-    <row r="759" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="759" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A759">
         <v>399238</v>
       </c>
@@ -34300,7 +34300,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="760" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="760" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A760">
         <v>399239</v>
       </c>
@@ -34330,7 +34330,7 @@
         <v>2521</v>
       </c>
     </row>
-    <row r="761" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="761" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A761">
         <v>399240</v>
       </c>
@@ -34350,7 +34350,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="762" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="762" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A762">
         <v>399241</v>
       </c>
@@ -34373,7 +34373,7 @@
         <v>2525</v>
       </c>
     </row>
-    <row r="763" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="763" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A763">
         <v>399242</v>
       </c>
@@ -34396,7 +34396,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="764" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="764" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A764">
         <v>399243</v>
       </c>
@@ -34416,7 +34416,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="765" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="765" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A765">
         <v>399244</v>
       </c>
@@ -34436,7 +34436,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="766" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="766" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A766">
         <v>399245</v>
       </c>
@@ -34465,7 +34465,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="767" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="767" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A767">
         <v>399246</v>
       </c>
@@ -34485,7 +34485,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="768" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="768" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A768">
         <v>399247</v>
       </c>
@@ -34519,7 +34519,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="769" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A769">
         <v>399248</v>
       </c>
@@ -34539,7 +34539,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="770" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A770">
         <v>399249</v>
       </c>
@@ -34565,7 +34565,7 @@
         <v>2548</v>
       </c>
     </row>
-    <row r="771" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="771" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A771">
         <v>399250</v>
       </c>
@@ -34595,7 +34595,7 @@
         <v>2552</v>
       </c>
     </row>
-    <row r="772" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A772">
         <v>399251</v>
       </c>
@@ -34615,7 +34615,7 @@
         <v>2555</v>
       </c>
     </row>
-    <row r="773" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A773">
         <v>399252</v>
       </c>
@@ -34641,7 +34641,7 @@
         <v>2558</v>
       </c>
     </row>
-    <row r="774" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A774">
         <v>399253</v>
       </c>
@@ -34661,7 +34661,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="775" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A775">
         <v>399254</v>
       </c>
@@ -34687,7 +34687,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="776" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A776">
         <v>399255</v>
       </c>
@@ -34707,7 +34707,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="777" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A777">
         <v>399256</v>
       </c>
@@ -34737,7 +34737,7 @@
         <v>2568</v>
       </c>
     </row>
-    <row r="778" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A778">
         <v>399257</v>
       </c>
@@ -34763,7 +34763,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="779" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A779">
         <v>399258</v>
       </c>
@@ -34783,7 +34783,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="780" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A780">
         <v>399259</v>
       </c>
@@ -34809,7 +34809,7 @@
         <v>2576</v>
       </c>
     </row>
-    <row r="781" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A781">
         <v>399260</v>
       </c>
@@ -34829,7 +34829,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="782" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A782">
         <v>399261</v>
       </c>
@@ -34855,7 +34855,7 @@
         <v>2582</v>
       </c>
     </row>
-    <row r="783" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A783">
         <v>399262</v>
       </c>
@@ -34887,7 +34887,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="784" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A784">
         <v>399263</v>
       </c>
@@ -34913,7 +34913,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="785" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A785">
         <v>399264</v>
       </c>
@@ -34936,7 +34936,7 @@
         <v>2592</v>
       </c>
     </row>
-    <row r="786" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A786">
         <v>399265</v>
       </c>
@@ -34962,7 +34962,7 @@
         <v>2596</v>
       </c>
     </row>
-    <row r="787" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A787">
         <v>399266</v>
       </c>
@@ -34993,7 +34993,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="788" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A788">
         <v>399267</v>
       </c>
@@ -35013,7 +35013,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="789" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A789">
         <v>399268</v>
       </c>
@@ -35045,7 +35045,7 @@
         <v>2605</v>
       </c>
     </row>
-    <row r="790" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A790">
         <v>399269</v>
       </c>
@@ -35071,7 +35071,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="791" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="791" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A791">
         <v>399270</v>
       </c>
@@ -35094,7 +35094,7 @@
         <v>2611</v>
       </c>
     </row>
-    <row r="792" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A792">
         <v>399271</v>
       </c>
@@ -35117,7 +35117,7 @@
         <v>2614</v>
       </c>
     </row>
-    <row r="793" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A793">
         <v>399272</v>
       </c>
@@ -35140,7 +35140,7 @@
         <v>2617</v>
       </c>
     </row>
-    <row r="794" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A794">
         <v>399273</v>
       </c>
@@ -35160,7 +35160,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="795" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A795">
         <v>399274</v>
       </c>
@@ -35189,7 +35189,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="796" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A796">
         <v>399275</v>
       </c>
@@ -35212,7 +35212,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="797" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A797">
         <v>399276</v>
       </c>
@@ -35232,7 +35232,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="798" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A798">
         <v>399277</v>
       </c>
@@ -35258,7 +35258,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="799" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A799">
         <v>399278</v>
       </c>
@@ -35288,7 +35288,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="800" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A800">
         <v>399279</v>
       </c>
@@ -35308,7 +35308,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="801" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A801">
         <v>399280</v>
       </c>
@@ -35334,7 +35334,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="802" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A802">
         <v>399281</v>
       </c>
@@ -35357,7 +35357,7 @@
         <v>2642</v>
       </c>
     </row>
-    <row r="803" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A803">
         <v>399282</v>
       </c>
@@ -35377,7 +35377,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="804" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A804">
         <v>399283</v>
       </c>
@@ -35403,7 +35403,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="805" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A805">
         <v>399284</v>
       </c>
@@ -35423,7 +35423,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="806" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A806">
         <v>399285</v>
       </c>
@@ -35455,7 +35455,7 @@
         <v>2654</v>
       </c>
     </row>
-    <row r="807" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A807">
         <v>399286</v>
       </c>
@@ -35475,7 +35475,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="808" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A808">
         <v>399287</v>
       </c>
@@ -35499,7 +35499,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="809" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A809">
         <v>399288</v>
       </c>
@@ -35519,7 +35519,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="810" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A810">
         <v>399289</v>
       </c>
@@ -35548,7 +35548,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="811" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A811">
         <v>399290</v>
       </c>
@@ -35574,7 +35574,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="812" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A812">
         <v>399291</v>
       </c>
@@ -35594,7 +35594,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="813" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A813">
         <v>399292</v>
       </c>
@@ -35627,7 +35627,7 @@
         <v>2671</v>
       </c>
     </row>
-    <row r="814" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A814">
         <v>399293</v>
       </c>
@@ -35647,7 +35647,7 @@
         <v>2674</v>
       </c>
     </row>
-    <row r="815" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A815">
         <v>399294</v>
       </c>
@@ -35673,7 +35673,7 @@
         <v>2677</v>
       </c>
     </row>
-    <row r="816" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A816">
         <v>399295</v>
       </c>
@@ -35693,7 +35693,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="817" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A817">
         <v>399296</v>
       </c>
@@ -35719,7 +35719,7 @@
         <v>2683</v>
       </c>
     </row>
-    <row r="818" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A818">
         <v>399297</v>
       </c>
@@ -35745,7 +35745,7 @@
         <v>2687</v>
       </c>
     </row>
-    <row r="819" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A819">
         <v>399298</v>
       </c>
@@ -35768,7 +35768,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="820" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A820">
         <v>399299</v>
       </c>
@@ -35798,7 +35798,7 @@
         <v>2694</v>
       </c>
     </row>
-    <row r="821" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A821">
         <v>399300</v>
       </c>
@@ -35821,7 +35821,7 @@
         <v>2697</v>
       </c>
     </row>
-    <row r="822" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A822">
         <v>399301</v>
       </c>
@@ -35847,7 +35847,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="823" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A823">
         <v>399302</v>
       </c>
@@ -35867,7 +35867,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="824" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A824">
         <v>399303</v>
       </c>
@@ -35893,7 +35893,7 @@
         <v>2707</v>
       </c>
     </row>
-    <row r="825" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A825">
         <v>399304</v>
       </c>
@@ -35919,7 +35919,7 @@
         <v>2711</v>
       </c>
     </row>
-    <row r="826" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A826">
         <v>399305</v>
       </c>
@@ -35942,7 +35942,7 @@
         <v>2714</v>
       </c>
     </row>
-    <row r="827" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="827" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A827">
         <v>399306</v>
       </c>
@@ -35968,7 +35968,7 @@
         <v>2718</v>
       </c>
     </row>
-    <row r="828" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A828">
         <v>399307</v>
       </c>
@@ -35994,7 +35994,7 @@
         <v>2722</v>
       </c>
     </row>
-    <row r="829" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="829" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A829">
         <v>399308</v>
       </c>
@@ -36023,7 +36023,7 @@
         <v>2727</v>
       </c>
     </row>
-    <row r="830" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A830">
         <v>399309</v>
       </c>
@@ -36043,7 +36043,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="831" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A831">
         <v>399310</v>
       </c>
@@ -36073,7 +36073,7 @@
         <v>2732</v>
       </c>
     </row>
-    <row r="832" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A832">
         <v>399311</v>
       </c>
@@ -36099,7 +36099,7 @@
         <v>2735</v>
       </c>
     </row>
-    <row r="833" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A833">
         <v>399312</v>
       </c>
@@ -36119,7 +36119,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="834" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A834">
         <v>399313</v>
       </c>
@@ -36149,7 +36149,7 @@
         <v>2740</v>
       </c>
     </row>
-    <row r="835" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A835">
         <v>399314</v>
       </c>
@@ -36169,7 +36169,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="836" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A836">
         <v>399315</v>
       </c>
@@ -36192,7 +36192,7 @@
         <v>2744</v>
       </c>
     </row>
-    <row r="837" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A837">
         <v>399316</v>
       </c>
@@ -36212,7 +36212,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="838" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A838">
         <v>399317</v>
       </c>
@@ -36238,7 +36238,7 @@
         <v>2749</v>
       </c>
     </row>
-    <row r="839" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A839">
         <v>399318</v>
       </c>
@@ -36264,7 +36264,7 @@
         <v>2752</v>
       </c>
     </row>
-    <row r="840" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A840">
         <v>399319</v>
       </c>
@@ -36287,7 +36287,7 @@
         <v>2755</v>
       </c>
     </row>
-    <row r="841" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A841">
         <v>399320</v>
       </c>
@@ -36310,7 +36310,7 @@
         <v>2758</v>
       </c>
     </row>
-    <row r="842" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A842">
         <v>399321</v>
       </c>
@@ -36333,7 +36333,7 @@
         <v>2761</v>
       </c>
     </row>
-    <row r="843" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A843">
         <v>399322</v>
       </c>
@@ -36353,7 +36353,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="844" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A844">
         <v>399323</v>
       </c>
@@ -36379,7 +36379,7 @@
         <v>2766</v>
       </c>
     </row>
-    <row r="845" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A845">
         <v>399324</v>
       </c>
@@ -36402,7 +36402,7 @@
         <v>2768</v>
       </c>
     </row>
-    <row r="846" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A846">
         <v>399325</v>
       </c>
@@ -36422,7 +36422,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="847" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A847">
         <v>399326</v>
       </c>
@@ -36452,7 +36452,7 @@
         <v>2773</v>
       </c>
     </row>
-    <row r="848" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A848">
         <v>399327</v>
       </c>
@@ -36472,7 +36472,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="849" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A849">
         <v>399328</v>
       </c>
@@ -36498,7 +36498,7 @@
         <v>2778</v>
       </c>
     </row>
-    <row r="850" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="850" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A850">
         <v>399329</v>
       </c>
@@ -36518,7 +36518,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="851" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A851">
         <v>399330</v>
       </c>
@@ -36541,7 +36541,7 @@
         <v>2782</v>
       </c>
     </row>
-    <row r="852" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="852" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A852">
         <v>399331</v>
       </c>
@@ -36564,7 +36564,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="853" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="853" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A853">
         <v>399332</v>
       </c>
@@ -36584,7 +36584,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="854" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="854" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A854">
         <v>399333</v>
       </c>
@@ -36610,7 +36610,7 @@
         <v>2789</v>
       </c>
     </row>
-    <row r="855" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="855" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A855">
         <v>399334</v>
       </c>
@@ -36636,7 +36636,7 @@
         <v>2793</v>
       </c>
     </row>
-    <row r="856" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="856" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A856">
         <v>399335</v>
       </c>
@@ -36662,7 +36662,7 @@
         <v>2797</v>
       </c>
     </row>
-    <row r="857" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A857">
         <v>399336</v>
       </c>
@@ -36692,7 +36692,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="858" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="858" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A858">
         <v>399337</v>
       </c>
@@ -36718,7 +36718,7 @@
         <v>2805</v>
       </c>
     </row>
-    <row r="859" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="859" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A859">
         <v>399338</v>
       </c>
@@ -36738,7 +36738,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="860" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="860" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A860">
         <v>399339</v>
       </c>
@@ -36764,7 +36764,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="861" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A861">
         <v>399340</v>
       </c>
@@ -36793,7 +36793,7 @@
         <v>2814</v>
       </c>
     </row>
-    <row r="862" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A862">
         <v>399341</v>
       </c>
@@ -36822,7 +36822,7 @@
         <v>2819</v>
       </c>
     </row>
-    <row r="863" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A863">
         <v>399342</v>
       </c>
@@ -36848,7 +36848,7 @@
         <v>2823</v>
       </c>
     </row>
-    <row r="864" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="864" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A864">
         <v>399343</v>
       </c>
@@ -36880,7 +36880,7 @@
         <v>2827</v>
       </c>
     </row>
-    <row r="865" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A865">
         <v>399344</v>
       </c>
@@ -36900,7 +36900,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="866" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A866">
         <v>399345</v>
       </c>
@@ -36923,7 +36923,7 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="867" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A867">
         <v>399346</v>
       </c>
@@ -36943,7 +36943,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="868" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A868">
         <v>399347</v>
       </c>
@@ -36966,7 +36966,7 @@
         <v>2835</v>
       </c>
     </row>
-    <row r="869" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A869">
         <v>399348</v>
       </c>
@@ -36989,7 +36989,7 @@
         <v>2838</v>
       </c>
     </row>
-    <row r="870" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A870">
         <v>399349</v>
       </c>
@@ -37016,7 +37016,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="871" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A871">
         <v>399350</v>
       </c>
@@ -37047,7 +37047,7 @@
         <v>2845</v>
       </c>
     </row>
-    <row r="872" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A872">
         <v>399351</v>
       </c>
@@ -37083,7 +37083,7 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="873" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A873">
         <v>399352</v>
       </c>
@@ -37106,7 +37106,7 @@
         <v>2853</v>
       </c>
     </row>
-    <row r="874" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A874">
         <v>399353</v>
       </c>
@@ -37126,7 +37126,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="875" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A875">
         <v>399354</v>
       </c>
@@ -37149,7 +37149,7 @@
         <v>2857</v>
       </c>
     </row>
-    <row r="876" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A876">
         <v>399355</v>
       </c>
@@ -37175,7 +37175,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="877" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A877">
         <v>399356</v>
       </c>
@@ -37208,7 +37208,7 @@
         <v>2866</v>
       </c>
     </row>
-    <row r="878" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A878">
         <v>399357</v>
       </c>
@@ -37234,7 +37234,7 @@
         <v>2870</v>
       </c>
     </row>
-    <row r="879" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A879">
         <v>399358</v>
       </c>
@@ -37257,7 +37257,7 @@
         <v>2873</v>
       </c>
     </row>
-    <row r="880" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A880">
         <v>399359</v>
       </c>
@@ -37283,7 +37283,7 @@
         <v>2877</v>
       </c>
     </row>
-    <row r="881" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A881">
         <v>399360</v>
       </c>
@@ -37309,7 +37309,7 @@
         <v>2881</v>
       </c>
     </row>
-    <row r="882" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A882">
         <v>399361</v>
       </c>
@@ -37335,7 +37335,7 @@
         <v>2885</v>
       </c>
     </row>
-    <row r="883" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A883">
         <v>399362</v>
       </c>
@@ -37361,7 +37361,7 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="884" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A884">
         <v>399363</v>
       </c>
@@ -37387,7 +37387,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="885" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A885">
         <v>399364</v>
       </c>
@@ -37407,7 +37407,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="886" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A886">
         <v>399365</v>
       </c>
@@ -37433,7 +37433,7 @@
         <v>2898</v>
       </c>
     </row>
-    <row r="887" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A887">
         <v>399366</v>
       </c>
@@ -37456,7 +37456,7 @@
         <v>2902</v>
       </c>
     </row>
-    <row r="888" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A888">
         <v>399367</v>
       </c>
@@ -37476,7 +37476,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="889" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A889">
         <v>399368</v>
       </c>
@@ -37496,7 +37496,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="890" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A890">
         <v>399369</v>
       </c>
@@ -37522,7 +37522,7 @@
         <v>2909</v>
       </c>
     </row>
-    <row r="891" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A891">
         <v>399370</v>
       </c>
@@ -37542,7 +37542,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="892" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A892">
         <v>399371</v>
       </c>
@@ -37568,7 +37568,7 @@
         <v>2915</v>
       </c>
     </row>
-    <row r="893" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A893">
         <v>399372</v>
       </c>
@@ -37594,7 +37594,7 @@
         <v>2919</v>
       </c>
     </row>
-    <row r="894" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A894">
         <v>399373</v>
       </c>
@@ -37617,7 +37617,7 @@
         <v>2922</v>
       </c>
     </row>
-    <row r="895" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A895">
         <v>399374</v>
       </c>
@@ -37646,7 +37646,7 @@
         <v>2927</v>
       </c>
     </row>
-    <row r="896" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A896">
         <v>399375</v>
       </c>
@@ -37672,7 +37672,7 @@
         <v>2919</v>
       </c>
     </row>
-    <row r="897" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A897">
         <v>399376</v>
       </c>
@@ -37695,7 +37695,7 @@
         <v>2933</v>
       </c>
     </row>
-    <row r="898" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A898">
         <v>399377</v>
       </c>
@@ -37721,7 +37721,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="899" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A899">
         <v>399378</v>
       </c>
@@ -37747,7 +37747,7 @@
         <v>2941</v>
       </c>
     </row>
-    <row r="900" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A900">
         <v>399379</v>
       </c>
@@ -37773,7 +37773,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="901" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A901">
         <v>399380</v>
       </c>
@@ -37799,7 +37799,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="902" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A902">
         <v>399381</v>
       </c>
@@ -37825,7 +37825,7 @@
         <v>2953</v>
       </c>
     </row>
-    <row r="903" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A903">
         <v>399382</v>
       </c>
@@ -37858,7 +37858,7 @@
         <v>2958</v>
       </c>
     </row>
-    <row r="904" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A904">
         <v>399383</v>
       </c>
@@ -37878,7 +37878,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="905" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A905">
         <v>399384</v>
       </c>
@@ -37908,7 +37908,7 @@
         <v>2963</v>
       </c>
     </row>
-    <row r="906" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A906">
         <v>399385</v>
       </c>
@@ -37928,7 +37928,7 @@
         <v>2966</v>
       </c>
     </row>
-    <row r="907" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A907">
         <v>399386</v>
       </c>
@@ -37954,7 +37954,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="908" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A908">
         <v>399387</v>
       </c>
@@ -37974,7 +37974,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="909" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A909">
         <v>399388</v>
       </c>
@@ -38000,7 +38000,7 @@
         <v>2974</v>
       </c>
     </row>
-    <row r="910" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A910">
         <v>399389</v>
       </c>
@@ -38026,7 +38026,7 @@
         <v>2978</v>
       </c>
     </row>
-    <row r="911" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A911">
         <v>399390</v>
       </c>
@@ -38052,7 +38052,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="912" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A912">
         <v>399391</v>
       </c>
@@ -38085,7 +38085,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="913" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A913">
         <v>399392</v>
       </c>
@@ -38114,7 +38114,7 @@
         <v>2992</v>
       </c>
     </row>
-    <row r="914" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A914">
         <v>399393</v>
       </c>
@@ -38134,7 +38134,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="915" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A915">
         <v>399394</v>
       </c>
@@ -38171,7 +38171,7 @@
         <v>2998</v>
       </c>
     </row>
-    <row r="916" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A916">
         <v>399395</v>
       </c>
@@ -38194,7 +38194,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="917" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A917">
         <v>399396</v>
       </c>
@@ -38214,7 +38214,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="918" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A918">
         <v>399397</v>
       </c>
@@ -38240,7 +38240,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row r="919" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A919">
         <v>399398</v>
       </c>
@@ -38260,7 +38260,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="920" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A920">
         <v>399399</v>
       </c>
@@ -38289,7 +38289,7 @@
         <v>3011</v>
       </c>
     </row>
-    <row r="921" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A921">
         <v>399400</v>
       </c>
@@ -38309,7 +38309,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="922" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A922">
         <v>399401</v>
       </c>
@@ -38335,7 +38335,7 @@
         <v>3016</v>
       </c>
     </row>
-    <row r="923" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A923">
         <v>399402</v>
       </c>
@@ -38355,7 +38355,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="924" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A924">
         <v>399403</v>
       </c>
@@ -38384,7 +38384,7 @@
         <v>3022</v>
       </c>
     </row>
-    <row r="925" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A925">
         <v>399404</v>
       </c>
@@ -38407,7 +38407,7 @@
         <v>3024</v>
       </c>
     </row>
-    <row r="926" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A926">
         <v>399405</v>
       </c>
@@ -38427,7 +38427,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="927" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A927">
         <v>399406</v>
       </c>
@@ -38453,7 +38453,7 @@
         <v>3029</v>
       </c>
     </row>
-    <row r="928" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A928">
         <v>399407</v>
       </c>
@@ -38473,7 +38473,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="929" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A929">
         <v>399408</v>
       </c>
@@ -38496,7 +38496,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="930" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="930" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A930">
         <v>399409</v>
       </c>
@@ -38528,7 +38528,7 @@
         <v>3038</v>
       </c>
     </row>
-    <row r="931" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A931">
         <v>399410</v>
       </c>
@@ -38548,7 +38548,7 @@
         <v>3041</v>
       </c>
     </row>
-    <row r="932" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="932" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A932">
         <v>399411</v>
       </c>
@@ -38574,7 +38574,7 @@
         <v>3044</v>
       </c>
     </row>
-    <row r="933" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="933" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A933">
         <v>399412</v>
       </c>
@@ -38597,7 +38597,7 @@
         <v>3046</v>
       </c>
     </row>
-    <row r="934" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="934" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A934">
         <v>399413</v>
       </c>
@@ -38628,7 +38628,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="935" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A935">
         <v>399414</v>
       </c>
@@ -38660,7 +38660,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="936" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="936" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A936">
         <v>399415</v>
       </c>
@@ -38689,7 +38689,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="937" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A937">
         <v>399416</v>
       </c>
@@ -38715,7 +38715,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="938" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="938" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A938">
         <v>399417</v>
       </c>
@@ -38744,7 +38744,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="939" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A939">
         <v>399418</v>
       </c>
@@ -38764,7 +38764,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="940" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A940">
         <v>399419</v>
       </c>
@@ -38787,7 +38787,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="941" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A941">
         <v>399420</v>
       </c>
@@ -38813,7 +38813,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="942" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A942">
         <v>399421</v>
       </c>
@@ -38839,7 +38839,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="943" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A943">
         <v>399422</v>
       </c>
@@ -38865,7 +38865,7 @@
         <v>3084</v>
       </c>
     </row>
-    <row r="944" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A944">
         <v>399423</v>
       </c>
@@ -38888,7 +38888,7 @@
         <v>3086</v>
       </c>
     </row>
-    <row r="945" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A945">
         <v>399424</v>
       </c>
@@ -38908,7 +38908,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="946" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A946">
         <v>399425</v>
       </c>
@@ -38935,7 +38935,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="947" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A947">
         <v>399426</v>
       </c>
@@ -38961,7 +38961,7 @@
         <v>3092</v>
       </c>
     </row>
-    <row r="948" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A948">
         <v>399427</v>
       </c>
@@ -38984,7 +38984,7 @@
         <v>3095</v>
       </c>
     </row>
-    <row r="949" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A949">
         <v>399428</v>
       </c>
@@ -39017,7 +39017,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="950" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A950">
         <v>399429</v>
       </c>
@@ -39046,7 +39046,7 @@
         <v>3105</v>
       </c>
     </row>
-    <row r="951" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A951">
         <v>399430</v>
       </c>
@@ -39072,7 +39072,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="952" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A952">
         <v>399431</v>
       </c>
@@ -39101,7 +39101,7 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="953" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A953">
         <v>399432</v>
       </c>
@@ -39127,7 +39127,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="954" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A954">
         <v>399433</v>
       </c>
@@ -39154,7 +39154,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="955" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="955" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A955">
         <v>399434</v>
       </c>
@@ -39189,7 +39189,7 @@
         <v>3126</v>
       </c>
     </row>
-    <row r="956" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="956" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A956">
         <v>399435</v>
       </c>
@@ -39209,7 +39209,7 @@
         <v>3129</v>
       </c>
     </row>
-    <row r="957" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="957" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A957">
         <v>399436</v>
       </c>
@@ -39232,7 +39232,7 @@
         <v>3131</v>
       </c>
     </row>
-    <row r="958" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="958" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A958">
         <v>399437</v>
       </c>
@@ -39258,7 +39258,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="959" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="959" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A959">
         <v>399438</v>
       </c>
@@ -39284,7 +39284,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="960" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="960" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A960">
         <v>399439</v>
       </c>
@@ -39313,7 +39313,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="961" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="961" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A961">
         <v>399440</v>
       </c>
@@ -39333,7 +39333,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="962" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="962" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A962">
         <v>399441</v>
       </c>
@@ -39362,7 +39362,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="963" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="963" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A963">
         <v>399442</v>
       </c>
@@ -39385,7 +39385,7 @@
         <v>3153</v>
       </c>
     </row>
-    <row r="964" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="964" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A964">
         <v>399443</v>
       </c>
@@ -39414,7 +39414,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="965" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A965">
         <v>399444</v>
       </c>
@@ -39437,7 +39437,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="966" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="966" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A966">
         <v>399445</v>
       </c>
@@ -39466,7 +39466,7 @@
         <v>3166</v>
       </c>
     </row>
-    <row r="967" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="967" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A967">
         <v>399446</v>
       </c>
@@ -39495,7 +39495,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="968" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="968" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A968">
         <v>399447</v>
       </c>
@@ -39518,7 +39518,7 @@
         <v>3173</v>
       </c>
     </row>
-    <row r="969" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A969">
         <v>399448</v>
       </c>
@@ -39551,7 +39551,7 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="970" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="970" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A970">
         <v>399449</v>
       </c>
@@ -39574,7 +39574,7 @@
         <v>3181</v>
       </c>
     </row>
-    <row r="971" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="971" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A971">
         <v>399450</v>
       </c>
@@ -39597,7 +39597,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="972" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="972" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A972">
         <v>399451</v>
       </c>
@@ -39620,7 +39620,7 @@
         <v>3187</v>
       </c>
     </row>
-    <row r="973" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="973" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A973">
         <v>399452</v>
       </c>
@@ -39646,7 +39646,7 @@
         <v>3191</v>
       </c>
     </row>
-    <row r="974" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="974" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A974">
         <v>399453</v>
       </c>
@@ -39669,7 +39669,7 @@
         <v>3194</v>
       </c>
     </row>
-    <row r="975" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A975">
         <v>399454</v>
       </c>
@@ -39692,7 +39692,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="976" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A976">
         <v>399455</v>
       </c>
@@ -39718,7 +39718,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="977" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="977" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A977">
         <v>399456</v>
       </c>
@@ -39744,7 +39744,7 @@
         <v>3205</v>
       </c>
     </row>
-    <row r="978" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="978" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A978">
         <v>399457</v>
       </c>
@@ -39767,7 +39767,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="979" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="979" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A979">
         <v>399458</v>
       </c>
@@ -39787,7 +39787,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="980" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="980" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A980">
         <v>399459</v>
       </c>
@@ -39813,7 +39813,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="981" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="981" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A981">
         <v>399460</v>
       </c>
@@ -39844,7 +39844,7 @@
         <v>3216</v>
       </c>
     </row>
-    <row r="982" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="982" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A982">
         <v>399461</v>
       </c>
@@ -39870,7 +39870,7 @@
         <v>3220</v>
       </c>
     </row>
-    <row r="983" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="983" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A983">
         <v>399462</v>
       </c>
@@ -39896,7 +39896,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="984" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="984" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A984">
         <v>399463</v>
       </c>
@@ -39925,7 +39925,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="985" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="985" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A985">
         <v>399464</v>
       </c>
@@ -39942,7 +39942,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="986" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="986" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A986">
         <v>399465</v>
       </c>
@@ -39962,7 +39962,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="987" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="987" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A987">
         <v>399466</v>
       </c>
@@ -39982,7 +39982,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="988" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="988" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A988">
         <v>399467</v>
       </c>
@@ -40008,7 +40008,7 @@
         <v>3236</v>
       </c>
     </row>
-    <row r="989" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="989" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A989">
         <v>399468</v>
       </c>
@@ -40031,7 +40031,7 @@
         <v>3238</v>
       </c>
     </row>
-    <row r="990" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="990" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A990">
         <v>399469</v>
       </c>
@@ -40051,7 +40051,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="991" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="991" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A991">
         <v>399470</v>
       </c>
@@ -40074,7 +40074,7 @@
         <v>3242</v>
       </c>
     </row>
-    <row r="992" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="992" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A992">
         <v>399471</v>
       </c>
@@ -40094,7 +40094,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="993" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="993" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A993">
         <v>399472</v>
       </c>
@@ -40117,7 +40117,7 @@
         <v>3246</v>
       </c>
     </row>
-    <row r="994" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="994" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A994">
         <v>399473</v>
       </c>
@@ -40134,7 +40134,7 @@
         <v>3247</v>
       </c>
     </row>
-    <row r="995" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="995" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A995">
         <v>399474</v>
       </c>
@@ -40154,7 +40154,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="996" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="996" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A996">
         <v>399475</v>
       </c>
@@ -40174,7 +40174,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="997" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="997" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A997">
         <v>399476</v>
       </c>

</xml_diff>